<commit_message>
Beginning of design doc, update of acquisitions
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Acquisitions.xlsx
+++ b/Inventory and Acquisitions/Master Acquisitions.xlsx
@@ -75,9 +75,6 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>81-GRM188R61A106KE9D</t>
-  </si>
-  <si>
     <t>GRM188R61A106KE69D</t>
   </si>
   <si>
@@ -126,10 +123,13 @@
     <t>81-GRM18R60J475KE19D</t>
   </si>
   <si>
-    <t>GRM188R60J475KE19D</t>
-  </si>
-  <si>
-    <t>0.061/0.035/--</t>
+    <t>81-GRM188R60J106ME47</t>
+  </si>
+  <si>
+    <t>GRM188R60J106ME47D</t>
+  </si>
+  <si>
+    <t>0.163/0.096/--</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -594,7 +594,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -617,48 +617,48 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
       </c>
       <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
         <v>20</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
       </c>
       <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
         <v>24</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>25</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>26</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -666,13 +666,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -681,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Just a few changes to suppliers/notes
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Acquisitions.xlsx
+++ b/Inventory and Acquisitions/Master Acquisitions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Last updated: Aug. 12/14</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>GRM188R61A106KE69D</t>
-  </si>
-  <si>
-    <t>0.096/0.056/--</t>
-  </si>
-  <si>
     <t>10 min.</t>
   </si>
   <si>
@@ -123,13 +117,22 @@
     <t>81-GRM18R60J475KE19D</t>
   </si>
   <si>
-    <t>81-GRM188R60J106ME47</t>
-  </si>
-  <si>
     <t>GRM188R60J106ME47D</t>
   </si>
   <si>
     <t>0.163/0.096/--</t>
+  </si>
+  <si>
+    <t>963-AMK107ABJ106MAHT</t>
+  </si>
+  <si>
+    <t>AMK107ABJ106MAHT</t>
+  </si>
+  <si>
+    <t>0.073/0.042/--</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
   </si>
 </sst>
 </file>
@@ -512,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +597,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -602,7 +605,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -620,45 +623,45 @@
         <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
       </c>
       <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -666,13 +669,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -681,16 +684,16 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
         <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on keeping things organized
Updates to acquisition list for RevB of micro board; update to inventory
to reflect what we have
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Acquisitions.xlsx
+++ b/Inventory and Acquisitions/Master Acquisitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>Updated by: Erik</t>
   </si>
@@ -58,6 +58,150 @@
   </si>
   <si>
     <t>Last updated:Sept. 23/14</t>
+  </si>
+  <si>
+    <t>~10</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>C203</t>
+  </si>
+  <si>
+    <t>SMD_0603</t>
+  </si>
+  <si>
+    <t>ROHS</t>
+  </si>
+  <si>
+    <t>~6</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>U101</t>
+  </si>
+  <si>
+    <t>TQFP ??</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>556-ATMEGA328P-AU</t>
+  </si>
+  <si>
+    <t>Atmel</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AU</t>
+  </si>
+  <si>
+    <t>3.64/2.74/2.58</t>
+  </si>
+  <si>
+    <t>compliant</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>16M</t>
+  </si>
+  <si>
+    <t>X101</t>
+  </si>
+  <si>
+    <t>CSTCE</t>
+  </si>
+  <si>
+    <t>??????Resonator</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>~14</t>
+  </si>
+  <si>
+    <t>R106,R107</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>R105,R108</t>
+  </si>
+  <si>
+    <t>~15</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>~4</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>595-LP2985-33DBVR</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>LP2985-33DBVR</t>
+  </si>
+  <si>
+    <t>0.578/0.43/0.317</t>
+  </si>
+  <si>
+    <t>81-CSTCE16M0V53-R0</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>CSTCE16M0V53-R0</t>
+  </si>
+  <si>
+    <t>0.434/0.35/--</t>
+  </si>
+  <si>
+    <t>Pin Headers</t>
+  </si>
+  <si>
+    <t>~5</t>
+  </si>
+  <si>
+    <t>517-9611106404AR</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>961110-6404-AR</t>
+  </si>
+  <si>
+    <t>--/0.437/0.412</t>
   </si>
 </sst>
 </file>
@@ -129,11 +273,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -438,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,44 +601,45 @@
     <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="25" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -524,8 +670,235 @@
       <c r="J8" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="K8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>180</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Order components for RevB Micro
Updates to acquisitions to reflect ordered components; added the order
to the expenses folder
</commit_message>
<xml_diff>
--- a/Inventory and Acquisitions/Master Acquisitions.xlsx
+++ b/Inventory and Acquisitions/Master Acquisitions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
   <si>
     <t>Updated by: Erik</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Pricing (10/100/500)</t>
   </si>
   <si>
-    <t>~10</t>
-  </si>
-  <si>
     <t>4.7u</t>
   </si>
   <si>
@@ -72,18 +69,12 @@
     <t>ROHS</t>
   </si>
   <si>
-    <t>~6</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>U101</t>
   </si>
   <si>
-    <t>TQFP ??</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
@@ -117,9 +108,6 @@
     <t>CSTCE</t>
   </si>
   <si>
-    <t>??????Resonator</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -129,9 +117,6 @@
     <t>R104</t>
   </si>
   <si>
-    <t>~14</t>
-  </si>
-  <si>
     <t>R106,R107</t>
   </si>
   <si>
@@ -144,15 +129,9 @@
     <t>R105,R108</t>
   </si>
   <si>
-    <t>~15</t>
-  </si>
-  <si>
     <t>Regulator</t>
   </si>
   <si>
-    <t>~4</t>
-  </si>
-  <si>
     <t>U103</t>
   </si>
   <si>
@@ -186,9 +165,6 @@
     <t>Pin Headers</t>
   </si>
   <si>
-    <t>~5</t>
-  </si>
-  <si>
     <t>517-9611106404AR</t>
   </si>
   <si>
@@ -204,10 +180,91 @@
     <t>Last updated: Oct. 21/14</t>
   </si>
   <si>
-    <t>LEDs</t>
-  </si>
-  <si>
-    <t>!!</t>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>LED5</t>
+  </si>
+  <si>
+    <t>710-150060RS75000</t>
+  </si>
+  <si>
+    <t>Wurth</t>
+  </si>
+  <si>
+    <t>150060RS75000</t>
+  </si>
+  <si>
+    <t>0.253/0.232/--</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>LED4</t>
+  </si>
+  <si>
+    <t>710-150060VS75000</t>
+  </si>
+  <si>
+    <t>150060VS75000</t>
+  </si>
+  <si>
+    <t>Resonator</t>
+  </si>
+  <si>
+    <t>TQFP_32</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>81-GRM18R60J475KE19D</t>
+  </si>
+  <si>
+    <t>GRM188R60J475KE19D</t>
+  </si>
+  <si>
+    <t>0.063/0.035/--</t>
+  </si>
+  <si>
+    <t>77-VJ0603Y103KXAAC</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>VJ0603Y103KXAAC</t>
+  </si>
+  <si>
+    <t>0.06/0.036/0.03</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-0-E3</t>
+  </si>
+  <si>
+    <t>CRCW06030000Z0EA</t>
+  </si>
+  <si>
+    <t>0.012/0.01/--</t>
+  </si>
+  <si>
+    <t>exemption</t>
+  </si>
+  <si>
+    <t>71-CRCW0603J-180-E3</t>
+  </si>
+  <si>
+    <t>CRCW0603180RJNEA</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-2.0K-E3</t>
+  </si>
+  <si>
+    <t>CRCW06032K00FKEA</t>
+  </si>
+  <si>
+    <t>0.016/0.012/--</t>
   </si>
 </sst>
 </file>
@@ -589,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +675,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -677,243 +734,392 @@
         <v>12</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>22</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="s">
+      <c r="K10" t="s">
         <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>51</v>
-      </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
       </c>
       <c r="C13">
         <v>180</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" t="s">
-        <v>50</v>
-      </c>
       <c r="K16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
       </c>
       <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
         <v>62</v>
       </c>
-      <c r="B18" t="s">
+      <c r="H19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" t="s">
         <v>63</v>
       </c>
-      <c r="C18" t="s">
-        <v>63</v>
+      <c r="J19" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>